<commit_message>
UI tweaks and data update
</commit_message>
<xml_diff>
--- a/23021-20230824-COORDINATES.xlsx
+++ b/23021-20230824-COORDINATES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ares\Hydrology\Hydrology Workspace\Nic\Projects\dam-it\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\nic\repos\dam-dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1C1612-F091-46D4-B3A5-CBA35E5158F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E1C683-B811-41F5-844E-5221D552AA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="2715" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01 23021-P" sheetId="1" r:id="rId1"/>
@@ -871,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I116"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="J107" sqref="J107"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="I119" sqref="I119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2850,104 +2850,223 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>1818765.95</v>
+        <v>1818764.4280000001</v>
       </c>
       <c r="B111">
-        <v>5578111.4199999999</v>
+        <v>5578108.6739999996</v>
       </c>
       <c r="C111">
-        <v>286.47199999999998</v>
+        <v>287.20499999999998</v>
       </c>
       <c r="E111">
-        <v>3.7240000000000002</v>
+        <v>1.123</v>
       </c>
       <c r="F111">
-        <v>51.486000000000004</v>
+        <v>48.885000000000005</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>1818766.76</v>
+        <v>1818764.024</v>
       </c>
       <c r="B112">
-        <v>5578114.3899999997</v>
+        <v>5578109.9699999997</v>
       </c>
       <c r="C112">
-        <v>285.73899999999998</v>
+        <v>286.97800000000001</v>
       </c>
       <c r="E112">
-        <v>3.0779999999999998</v>
+        <v>1.3580000000000001</v>
       </c>
       <c r="F112">
-        <v>54.564000000000007</v>
+        <v>50.243000000000002</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>1818767.41</v>
+        <v>1818763.557</v>
       </c>
       <c r="B113">
-        <v>5578115.5300000003</v>
+        <v>5578111.71</v>
       </c>
       <c r="C113">
-        <v>285.53800000000001</v>
+        <v>286.57400000000001</v>
       </c>
       <c r="E113">
-        <v>1.3120000000000001</v>
+        <v>1.802</v>
       </c>
       <c r="F113">
-        <v>55.876000000000005</v>
+        <v>52.045000000000002</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>1818767.66</v>
+        <v>1818762.865</v>
       </c>
       <c r="B114">
-        <v>5578117.8799999999</v>
+        <v>5578113.3329999996</v>
       </c>
       <c r="C114">
-        <v>285.464</v>
+        <v>286.03699999999998</v>
       </c>
       <c r="E114">
-        <v>2.363</v>
+        <v>1.764</v>
       </c>
       <c r="F114">
-        <v>58.239000000000004</v>
+        <v>53.809000000000005</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>1818768.14</v>
+        <v>1818762.585</v>
       </c>
       <c r="B115">
-        <v>5578118.2300000004</v>
+        <v>5578114.5259999996</v>
       </c>
       <c r="C115">
-        <v>285.58199999999999</v>
+        <v>285.64499999999998</v>
       </c>
       <c r="E115">
-        <v>0.59399999999999997</v>
+        <v>1.2250000000000001</v>
       </c>
       <c r="F115">
-        <v>58.833000000000006</v>
+        <v>55.034000000000006</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>1818768.08</v>
+        <v>1818762.3019999999</v>
       </c>
       <c r="B116">
-        <v>5578119.6900000004</v>
+        <v>5578116.159</v>
       </c>
       <c r="C116">
-        <v>285.471</v>
+        <v>285.61799999999999</v>
       </c>
       <c r="E116">
-        <v>1.4610000000000001</v>
+        <v>1.657</v>
       </c>
       <c r="F116">
-        <v>60.294000000000004</v>
+        <v>56.691000000000003</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>1818761.8430000001</v>
+      </c>
+      <c r="B117">
+        <v>5578118.1330000004</v>
+      </c>
+      <c r="C117">
+        <v>285.58800000000002</v>
+      </c>
+      <c r="E117">
+        <v>2.0270000000000001</v>
+      </c>
+      <c r="F117">
+        <v>58.718000000000004</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>1818761.379</v>
+      </c>
+      <c r="B118">
+        <v>5578119.4029999999</v>
+      </c>
+      <c r="C118">
+        <v>285.59199999999998</v>
+      </c>
+      <c r="E118">
+        <v>1.3520000000000001</v>
+      </c>
+      <c r="F118">
+        <v>60.07</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>1818761.3370000001</v>
+      </c>
+      <c r="B119">
+        <v>5578119.8150000004</v>
+      </c>
+      <c r="C119">
+        <v>285.875</v>
+      </c>
+      <c r="E119">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="F119">
+        <v>60.484000000000002</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>1818761.2039999999</v>
+      </c>
+      <c r="B120">
+        <v>5578120.307</v>
+      </c>
+      <c r="C120">
+        <v>286.38600000000002</v>
+      </c>
+      <c r="E120">
+        <v>0.51</v>
+      </c>
+      <c r="F120">
+        <v>60.994</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>1818761.3430000001</v>
+      </c>
+      <c r="B121">
+        <v>5578120.665</v>
+      </c>
+      <c r="C121">
+        <v>287.101</v>
+      </c>
+      <c r="E121">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="F121">
+        <v>61.378</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>1818760.024</v>
+      </c>
+      <c r="B122">
+        <v>5578121.9440000001</v>
+      </c>
+      <c r="C122">
+        <v>287.41500000000002</v>
+      </c>
+      <c r="E122">
+        <v>1.837</v>
+      </c>
+      <c r="F122">
+        <v>63.215000000000003</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>1818758.6529999999</v>
+      </c>
+      <c r="B123">
+        <v>5578124.7249999996</v>
+      </c>
+      <c r="C123">
+        <v>288.31299999999999</v>
+      </c>
+      <c r="E123">
+        <v>3.101</v>
+      </c>
+      <c r="F123">
+        <v>66.316000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove docker stuff, added tawataia dam
</commit_message>
<xml_diff>
--- a/23021-20230824-COORDINATES.xlsx
+++ b/23021-20230824-COORDINATES.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\nic\repos\dam-dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E1C683-B811-41F5-844E-5221D552AA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47457BA-1FE4-4410-9867-6CA298B9209B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01 23021-P" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="14">
   <si>
     <t>X</t>
   </si>
@@ -59,6 +72,9 @@
   </si>
   <si>
     <t>gap between points</t>
+  </si>
+  <si>
+    <t>TAWATAIA DAM</t>
   </si>
 </sst>
 </file>
@@ -871,16 +887,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:I161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="I119" sqref="I119"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="R89" sqref="R89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
@@ -2688,7 +2704,7 @@
         <v>2</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>12</v>
@@ -2882,7 +2898,7 @@
         <v>50.243000000000002</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>1818763.557</v>
       </c>
@@ -2899,7 +2915,7 @@
         <v>52.045000000000002</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>1818762.865</v>
       </c>
@@ -2916,7 +2932,7 @@
         <v>53.809000000000005</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>1818762.585</v>
       </c>
@@ -2933,7 +2949,7 @@
         <v>55.034000000000006</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>1818762.3019999999</v>
       </c>
@@ -2950,7 +2966,7 @@
         <v>56.691000000000003</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>1818761.8430000001</v>
       </c>
@@ -2967,7 +2983,7 @@
         <v>58.718000000000004</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>1818761.379</v>
       </c>
@@ -2984,7 +3000,7 @@
         <v>60.07</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>1818761.3370000001</v>
       </c>
@@ -3001,7 +3017,7 @@
         <v>60.484000000000002</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>1818761.2039999999</v>
       </c>
@@ -3018,7 +3034,7 @@
         <v>60.994</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>1818761.3430000001</v>
       </c>
@@ -3035,7 +3051,7 @@
         <v>61.378</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>1818760.024</v>
       </c>
@@ -3052,7 +3068,7 @@
         <v>63.215000000000003</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>1818758.6529999999</v>
       </c>
@@ -3067,6 +3083,744 @@
       </c>
       <c r="F123">
         <v>66.316000000000003</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>0</v>
+      </c>
+      <c r="B124" t="s">
+        <v>1</v>
+      </c>
+      <c r="C124" t="s">
+        <v>2</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G124" t="s">
+        <v>10</v>
+      </c>
+      <c r="H124" t="s">
+        <v>8</v>
+      </c>
+      <c r="I124" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>1837443.1</v>
+      </c>
+      <c r="B125">
+        <v>5496185.5999999996</v>
+      </c>
+      <c r="C125">
+        <v>171.98400000000001</v>
+      </c>
+      <c r="F125">
+        <v>0</v>
+      </c>
+      <c r="G125">
+        <f>I125+8</f>
+        <v>176.98</v>
+      </c>
+      <c r="H125">
+        <f>I125+4</f>
+        <v>172.98</v>
+      </c>
+      <c r="I125">
+        <v>168.98</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>1837447.15</v>
+      </c>
+      <c r="B126">
+        <v>5496194.8399999999</v>
+      </c>
+      <c r="C126">
+        <v>171.976</v>
+      </c>
+      <c r="E126">
+        <f>SQRT((A126-A125)^2 + (B125-B126)^2)</f>
+        <v>10.088612392327393</v>
+      </c>
+      <c r="F126">
+        <f>F125+E126</f>
+        <v>10.088612392327393</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>1837451.26</v>
+      </c>
+      <c r="B127">
+        <v>5496204.3499999996</v>
+      </c>
+      <c r="C127">
+        <v>171.989</v>
+      </c>
+      <c r="E127">
+        <f>SQRT((A127-A126)^2 + (B126-B127)^2)</f>
+        <v>10.36012548170102</v>
+      </c>
+      <c r="F127">
+        <f t="shared" ref="F127:F161" si="0">F126+E127</f>
+        <v>20.448737874028414</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>1837455.19</v>
+      </c>
+      <c r="B128">
+        <v>5496213.7999999998</v>
+      </c>
+      <c r="C128">
+        <v>172.02600000000001</v>
+      </c>
+      <c r="E128">
+        <f t="shared" ref="E128:E161" si="1">SQRT((A128-A127)^2 + (B127-B128)^2)</f>
+        <v>10.234617726276248</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="0"/>
+        <v>30.683355600304662</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>1837459.09</v>
+      </c>
+      <c r="B129">
+        <v>5496223.3099999996</v>
+      </c>
+      <c r="C129">
+        <v>172.04</v>
+      </c>
+      <c r="E129">
+        <f t="shared" si="1"/>
+        <v>10.278623448538152</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="0"/>
+        <v>40.961979048842814</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>1837463.07</v>
+      </c>
+      <c r="B130">
+        <v>5496233.0599999996</v>
+      </c>
+      <c r="C130">
+        <v>172.078</v>
+      </c>
+      <c r="E130">
+        <f t="shared" si="1"/>
+        <v>10.531044582559307</v>
+      </c>
+      <c r="F130">
+        <f t="shared" si="0"/>
+        <v>51.493023631402124</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>1837466.97</v>
+      </c>
+      <c r="B131">
+        <v>5496243.2699999996</v>
+      </c>
+      <c r="C131">
+        <v>172.119</v>
+      </c>
+      <c r="E131">
+        <f t="shared" si="1"/>
+        <v>10.929505935700519</v>
+      </c>
+      <c r="F131">
+        <f t="shared" si="0"/>
+        <v>62.422529567102643</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>1837470.37</v>
+      </c>
+      <c r="B132">
+        <v>5496253.1900000004</v>
+      </c>
+      <c r="C132">
+        <v>172.14500000000001</v>
+      </c>
+      <c r="E132">
+        <f t="shared" si="1"/>
+        <v>10.486486543068139</v>
+      </c>
+      <c r="F132">
+        <f t="shared" si="0"/>
+        <v>72.909016110170782</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>1837473.48</v>
+      </c>
+      <c r="B133">
+        <v>5496263.2000000002</v>
+      </c>
+      <c r="C133">
+        <v>172.148</v>
+      </c>
+      <c r="E133">
+        <f t="shared" si="1"/>
+        <v>10.481994084844457</v>
+      </c>
+      <c r="F133">
+        <f t="shared" si="0"/>
+        <v>83.391010195015241</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>1837476.06</v>
+      </c>
+      <c r="B134">
+        <v>5496273.5</v>
+      </c>
+      <c r="C134">
+        <v>172.18299999999999</v>
+      </c>
+      <c r="E134">
+        <f t="shared" si="1"/>
+        <v>10.618210771902552</v>
+      </c>
+      <c r="F134">
+        <f t="shared" si="0"/>
+        <v>94.009220966917795</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>1837478.42</v>
+      </c>
+      <c r="B135">
+        <v>5496283.8899999997</v>
+      </c>
+      <c r="C135">
+        <v>172.21700000000001</v>
+      </c>
+      <c r="E135">
+        <f t="shared" si="1"/>
+        <v>10.654656258763938</v>
+      </c>
+      <c r="F135">
+        <f t="shared" si="0"/>
+        <v>104.66387722568173</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>1837480.01</v>
+      </c>
+      <c r="B136">
+        <v>5496294.7699999996</v>
+      </c>
+      <c r="C136">
+        <v>172.203</v>
+      </c>
+      <c r="E136">
+        <f t="shared" si="1"/>
+        <v>10.995567288586555</v>
+      </c>
+      <c r="F136">
+        <f t="shared" si="0"/>
+        <v>115.65944451426829</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>1837481.36</v>
+      </c>
+      <c r="B137">
+        <v>5496305.5700000003</v>
+      </c>
+      <c r="C137">
+        <v>172.17400000000001</v>
+      </c>
+      <c r="E137">
+        <f t="shared" si="1"/>
+        <v>10.884047960953898</v>
+      </c>
+      <c r="F137">
+        <f t="shared" si="0"/>
+        <v>126.54349247522218</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>1837482.11</v>
+      </c>
+      <c r="B138">
+        <v>5496315.9500000002</v>
+      </c>
+      <c r="C138">
+        <v>172.12799999999999</v>
+      </c>
+      <c r="E138">
+        <f t="shared" si="1"/>
+        <v>10.407060103491277</v>
+      </c>
+      <c r="F138">
+        <f t="shared" si="0"/>
+        <v>136.95055257871346</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>1837483.51</v>
+      </c>
+      <c r="B139">
+        <v>5496328.2300000004</v>
+      </c>
+      <c r="C139">
+        <v>172.17</v>
+      </c>
+      <c r="E139">
+        <f t="shared" si="1"/>
+        <v>12.359546917510517</v>
+      </c>
+      <c r="F139">
+        <f t="shared" si="0"/>
+        <v>149.31009949622398</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>1837484.22</v>
+      </c>
+      <c r="B140">
+        <v>5496338.5</v>
+      </c>
+      <c r="C140">
+        <v>172.33500000000001</v>
+      </c>
+      <c r="E140">
+        <f t="shared" si="1"/>
+        <v>10.294513101199348</v>
+      </c>
+      <c r="F140">
+        <f t="shared" si="0"/>
+        <v>159.60461259742334</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>1837484.94</v>
+      </c>
+      <c r="B141">
+        <v>5496348.2300000004</v>
+      </c>
+      <c r="C141">
+        <v>172.64</v>
+      </c>
+      <c r="E141">
+        <f t="shared" si="1"/>
+        <v>9.7566028928443664</v>
+      </c>
+      <c r="F141">
+        <f t="shared" si="0"/>
+        <v>169.36121549026771</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>1837485.49</v>
+      </c>
+      <c r="B142">
+        <v>5496358.3799999999</v>
+      </c>
+      <c r="C142">
+        <v>173.21799999999999</v>
+      </c>
+      <c r="E142">
+        <f t="shared" si="1"/>
+        <v>10.164890554684183</v>
+      </c>
+      <c r="F142">
+        <f t="shared" si="0"/>
+        <v>179.52610604495189</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>1837486.58</v>
+      </c>
+      <c r="B143">
+        <v>5496368.5800000001</v>
+      </c>
+      <c r="C143">
+        <v>174.018</v>
+      </c>
+      <c r="E143">
+        <f t="shared" si="1"/>
+        <v>10.258074868316301</v>
+      </c>
+      <c r="F143">
+        <f t="shared" si="0"/>
+        <v>189.78418091326819</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>1837487.59</v>
+      </c>
+      <c r="B144">
+        <v>5496378.7000000002</v>
+      </c>
+      <c r="C144">
+        <v>174.75800000000001</v>
+      </c>
+      <c r="E144">
+        <f t="shared" si="1"/>
+        <v>10.170275315952898</v>
+      </c>
+      <c r="F144">
+        <f t="shared" si="0"/>
+        <v>199.95445622922108</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>1837489.15</v>
+      </c>
+      <c r="B145">
+        <v>5496388.9100000001</v>
+      </c>
+      <c r="C145">
+        <v>175.10599999999999</v>
+      </c>
+      <c r="E145">
+        <f t="shared" si="1"/>
+        <v>10.328489724964014</v>
+      </c>
+      <c r="F145">
+        <f t="shared" si="0"/>
+        <v>210.2829459541851</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>1837490.7</v>
+      </c>
+      <c r="B146">
+        <v>5496399.6699999999</v>
+      </c>
+      <c r="C146">
+        <v>174.86600000000001</v>
+      </c>
+      <c r="E146">
+        <f t="shared" si="1"/>
+        <v>10.871067104720414</v>
+      </c>
+      <c r="F146">
+        <f t="shared" si="0"/>
+        <v>221.15401305890552</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>1837491.89</v>
+      </c>
+      <c r="B147">
+        <v>5496409.7000000002</v>
+      </c>
+      <c r="C147">
+        <v>174.44499999999999</v>
+      </c>
+      <c r="E147">
+        <f t="shared" si="1"/>
+        <v>10.100346528961175</v>
+      </c>
+      <c r="F147">
+        <f t="shared" si="0"/>
+        <v>231.2543595878667</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>1837493.05</v>
+      </c>
+      <c r="B148">
+        <v>5496419.4699999997</v>
+      </c>
+      <c r="C148">
+        <v>174.096</v>
+      </c>
+      <c r="E148">
+        <f t="shared" si="1"/>
+        <v>9.8386228706872725</v>
+      </c>
+      <c r="F148">
+        <f t="shared" si="0"/>
+        <v>241.09298245855396</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>1837493.96</v>
+      </c>
+      <c r="B149">
+        <v>5496429.5</v>
+      </c>
+      <c r="C149">
+        <v>173.79300000000001</v>
+      </c>
+      <c r="E149">
+        <f t="shared" si="1"/>
+        <v>10.071196552797414</v>
+      </c>
+      <c r="F149">
+        <f t="shared" si="0"/>
+        <v>251.16417901135137</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>1837494.77</v>
+      </c>
+      <c r="B150">
+        <v>5496439.6200000001</v>
+      </c>
+      <c r="C150">
+        <v>173.52</v>
+      </c>
+      <c r="E150">
+        <f t="shared" si="1"/>
+        <v>10.152364256780414</v>
+      </c>
+      <c r="F150">
+        <f t="shared" si="0"/>
+        <v>261.3165432681318</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>1837495.48</v>
+      </c>
+      <c r="B151">
+        <v>5496449.9299999997</v>
+      </c>
+      <c r="C151">
+        <v>173.31800000000001</v>
+      </c>
+      <c r="E151">
+        <f t="shared" si="1"/>
+        <v>10.334418222207644</v>
+      </c>
+      <c r="F151">
+        <f t="shared" si="0"/>
+        <v>271.65096149033945</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>1837496.2</v>
+      </c>
+      <c r="B152">
+        <v>5496459.96</v>
+      </c>
+      <c r="C152">
+        <v>173.16200000000001</v>
+      </c>
+      <c r="E152">
+        <f t="shared" si="1"/>
+        <v>10.055809266547911</v>
+      </c>
+      <c r="F152">
+        <f t="shared" si="0"/>
+        <v>281.70677075688735</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>1837496.83</v>
+      </c>
+      <c r="B153">
+        <v>5496469.9900000002</v>
+      </c>
+      <c r="C153">
+        <v>172.958</v>
+      </c>
+      <c r="E153">
+        <f t="shared" si="1"/>
+        <v>10.049766166701771</v>
+      </c>
+      <c r="F153">
+        <f t="shared" si="0"/>
+        <v>291.75653692358912</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>1837497.45</v>
+      </c>
+      <c r="B154">
+        <v>5496479.96</v>
+      </c>
+      <c r="C154">
+        <v>172.77600000000001</v>
+      </c>
+      <c r="E154">
+        <f t="shared" si="1"/>
+        <v>9.9892592315271358</v>
+      </c>
+      <c r="F154">
+        <f t="shared" si="0"/>
+        <v>301.74579615511624</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>1837498.13</v>
+      </c>
+      <c r="B155">
+        <v>5496490.1100000003</v>
+      </c>
+      <c r="C155">
+        <v>172.57900000000001</v>
+      </c>
+      <c r="E155">
+        <f t="shared" si="1"/>
+        <v>10.172752823472793</v>
+      </c>
+      <c r="F155">
+        <f t="shared" si="0"/>
+        <v>311.91854897858906</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>1837498.86</v>
+      </c>
+      <c r="B156">
+        <v>5496500.4500000002</v>
+      </c>
+      <c r="C156">
+        <v>172.441</v>
+      </c>
+      <c r="E156">
+        <f t="shared" si="1"/>
+        <v>10.365736828476361</v>
+      </c>
+      <c r="F156">
+        <f t="shared" si="0"/>
+        <v>322.28428580706543</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>1837499.64</v>
+      </c>
+      <c r="B157">
+        <v>5496510.7999999998</v>
+      </c>
+      <c r="C157">
+        <v>172.37</v>
+      </c>
+      <c r="E157">
+        <f t="shared" si="1"/>
+        <v>10.379349690224769</v>
+      </c>
+      <c r="F157">
+        <f t="shared" si="0"/>
+        <v>332.66363549729022</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>1837500.38</v>
+      </c>
+      <c r="B158">
+        <v>5496521.29</v>
+      </c>
+      <c r="C158">
+        <v>172.333</v>
+      </c>
+      <c r="E158">
+        <f t="shared" si="1"/>
+        <v>10.516068657282322</v>
+      </c>
+      <c r="F158">
+        <f t="shared" si="0"/>
+        <v>343.17970415457256</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>1837501.21</v>
+      </c>
+      <c r="B159">
+        <v>5496531.6100000003</v>
+      </c>
+      <c r="C159">
+        <v>172.37100000000001</v>
+      </c>
+      <c r="E159">
+        <f t="shared" si="1"/>
+        <v>10.353323138310467</v>
+      </c>
+      <c r="F159">
+        <f t="shared" si="0"/>
+        <v>353.53302729288305</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>1837501.9</v>
+      </c>
+      <c r="B160">
+        <v>5496541.6299999999</v>
+      </c>
+      <c r="C160">
+        <v>172.43299999999999</v>
+      </c>
+      <c r="E160">
+        <f t="shared" si="1"/>
+        <v>10.043729386585657</v>
+      </c>
+      <c r="F160">
+        <f t="shared" si="0"/>
+        <v>363.5767566794687</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>1837502.51</v>
+      </c>
+      <c r="B161">
+        <v>5496552.0800000001</v>
+      </c>
+      <c r="C161">
+        <v>172.54300000000001</v>
+      </c>
+      <c r="E161">
+        <f t="shared" si="1"/>
+        <v>10.467788687398018</v>
+      </c>
+      <c r="F161">
+        <f t="shared" si="0"/>
+        <v>374.04454536686671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>